<commit_message>
all MLC and FIO data
</commit_message>
<xml_diff>
--- a/Project3/ACS-Project3-MLC_Data.xlsx
+++ b/Project3/ACS-Project3-MLC_Data.xlsx
@@ -212,11 +212,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1271094960"/>
-        <c:axId val="413516670"/>
+        <c:axId val="1598778684"/>
+        <c:axId val="2062386367"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1271094960"/>
+        <c:axId val="1598778684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -268,10 +268,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413516670"/>
+        <c:crossAx val="2062386367"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="413516670"/>
+        <c:axId val="2062386367"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -346,7 +346,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1271094960"/>
+        <c:crossAx val="1598778684"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -438,11 +438,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="127253041"/>
-        <c:axId val="1793644897"/>
+        <c:axId val="822240808"/>
+        <c:axId val="337394280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127253041"/>
+        <c:axId val="822240808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,10 +494,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1793644897"/>
+        <c:crossAx val="337394280"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1793644897"/>
+        <c:axId val="337394280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,7 +572,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127253041"/>
+        <c:crossAx val="822240808"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -664,11 +664,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1094792759"/>
-        <c:axId val="1624939959"/>
+        <c:axId val="1245652699"/>
+        <c:axId val="469373097"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1094792759"/>
+        <c:axId val="1245652699"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,10 +720,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1624939959"/>
+        <c:crossAx val="469373097"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1624939959"/>
+        <c:axId val="469373097"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,7 +798,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1094792759"/>
+        <c:crossAx val="1245652699"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -890,11 +890,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="851432159"/>
-        <c:axId val="531973128"/>
+        <c:axId val="213867465"/>
+        <c:axId val="819147124"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="851432159"/>
+        <c:axId val="213867465"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,10 +946,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531973128"/>
+        <c:crossAx val="819147124"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="531973128"/>
+        <c:axId val="819147124"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1024,7 +1024,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="851432159"/>
+        <c:crossAx val="213867465"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1116,11 +1116,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="851541226"/>
-        <c:axId val="2092341194"/>
+        <c:axId val="1472159165"/>
+        <c:axId val="78845088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="851541226"/>
+        <c:axId val="1472159165"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1172,10 +1172,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2092341194"/>
+        <c:crossAx val="78845088"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092341194"/>
+        <c:axId val="78845088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,7 +1250,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="851541226"/>
+        <c:crossAx val="1472159165"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1342,11 +1342,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1720284409"/>
-        <c:axId val="1108976896"/>
+        <c:axId val="1297258396"/>
+        <c:axId val="1403859154"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1720284409"/>
+        <c:axId val="1297258396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1398,10 +1398,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1108976896"/>
+        <c:crossAx val="1403859154"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1108976896"/>
+        <c:axId val="1403859154"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,7 +1476,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1720284409"/>
+        <c:crossAx val="1297258396"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1568,11 +1568,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1821597530"/>
-        <c:axId val="848674371"/>
+        <c:axId val="1875597999"/>
+        <c:axId val="2052719585"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1821597530"/>
+        <c:axId val="1875597999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1624,10 +1624,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="848674371"/>
+        <c:crossAx val="2052719585"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="848674371"/>
+        <c:axId val="2052719585"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,7 +1702,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1821597530"/>
+        <c:crossAx val="1875597999"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1794,11 +1794,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="599480555"/>
-        <c:axId val="605549219"/>
+        <c:axId val="421906695"/>
+        <c:axId val="1589429978"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="599480555"/>
+        <c:axId val="421906695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1850,10 +1850,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="605549219"/>
+        <c:crossAx val="1589429978"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="605549219"/>
+        <c:axId val="1589429978"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1928,7 +1928,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="599480555"/>
+        <c:crossAx val="421906695"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2020,11 +2020,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1078544776"/>
-        <c:axId val="2040559875"/>
+        <c:axId val="689661435"/>
+        <c:axId val="1585372172"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1078544776"/>
+        <c:axId val="689661435"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2076,10 +2076,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2040559875"/>
+        <c:crossAx val="1585372172"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2040559875"/>
+        <c:axId val="1585372172"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,7 +2154,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078544776"/>
+        <c:crossAx val="689661435"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2246,11 +2246,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1478806017"/>
-        <c:axId val="1173164625"/>
+        <c:axId val="1327371287"/>
+        <c:axId val="1731031497"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1478806017"/>
+        <c:axId val="1327371287"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2302,10 +2302,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1173164625"/>
+        <c:crossAx val="1731031497"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1173164625"/>
+        <c:axId val="1731031497"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2380,7 +2380,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1478806017"/>
+        <c:crossAx val="1327371287"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2472,11 +2472,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1712605278"/>
-        <c:axId val="276795401"/>
+        <c:axId val="758524085"/>
+        <c:axId val="1563442419"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1712605278"/>
+        <c:axId val="758524085"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2528,10 +2528,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276795401"/>
+        <c:crossAx val="1563442419"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="276795401"/>
+        <c:axId val="1563442419"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2606,7 +2606,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1712605278"/>
+        <c:crossAx val="758524085"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2698,11 +2698,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1049757823"/>
-        <c:axId val="480617923"/>
+        <c:axId val="1671344514"/>
+        <c:axId val="1128597969"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1049757823"/>
+        <c:axId val="1671344514"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2754,10 +2754,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480617923"/>
+        <c:crossAx val="1128597969"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="480617923"/>
+        <c:axId val="1128597969"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2832,7 +2832,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1049757823"/>
+        <c:crossAx val="1671344514"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2924,11 +2924,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="407549740"/>
-        <c:axId val="442943984"/>
+        <c:axId val="898706146"/>
+        <c:axId val="524513056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="407549740"/>
+        <c:axId val="898706146"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2980,10 +2980,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442943984"/>
+        <c:crossAx val="524513056"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442943984"/>
+        <c:axId val="524513056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3058,7 +3058,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407549740"/>
+        <c:crossAx val="898706146"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3150,11 +3150,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1317089719"/>
-        <c:axId val="1092161002"/>
+        <c:axId val="119087386"/>
+        <c:axId val="1203341499"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1317089719"/>
+        <c:axId val="119087386"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3206,10 +3206,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1092161002"/>
+        <c:crossAx val="1203341499"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1092161002"/>
+        <c:axId val="1203341499"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3284,7 +3284,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1317089719"/>
+        <c:crossAx val="119087386"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3376,11 +3376,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="908077536"/>
-        <c:axId val="523253625"/>
+        <c:axId val="604466444"/>
+        <c:axId val="1052609574"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="908077536"/>
+        <c:axId val="604466444"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3432,10 +3432,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523253625"/>
+        <c:crossAx val="1052609574"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523253625"/>
+        <c:axId val="1052609574"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3510,7 +3510,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="908077536"/>
+        <c:crossAx val="604466444"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3602,11 +3602,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2003485575"/>
-        <c:axId val="185244889"/>
+        <c:axId val="349680403"/>
+        <c:axId val="1839123488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2003485575"/>
+        <c:axId val="349680403"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3658,10 +3658,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185244889"/>
+        <c:crossAx val="1839123488"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185244889"/>
+        <c:axId val="1839123488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3736,7 +3736,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2003485575"/>
+        <c:crossAx val="349680403"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3828,11 +3828,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1710552025"/>
-        <c:axId val="933905296"/>
+        <c:axId val="878690946"/>
+        <c:axId val="81817684"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1710552025"/>
+        <c:axId val="878690946"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3884,10 +3884,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="933905296"/>
+        <c:crossAx val="81817684"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="933905296"/>
+        <c:axId val="81817684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3962,7 +3962,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1710552025"/>
+        <c:crossAx val="878690946"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4054,11 +4054,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="559512514"/>
-        <c:axId val="366800890"/>
+        <c:axId val="1853776913"/>
+        <c:axId val="1338849546"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="559512514"/>
+        <c:axId val="1853776913"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4110,10 +4110,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366800890"/>
+        <c:crossAx val="1338849546"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="366800890"/>
+        <c:axId val="1338849546"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4188,7 +4188,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="559512514"/>
+        <c:crossAx val="1853776913"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4280,11 +4280,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1556014590"/>
-        <c:axId val="787541410"/>
+        <c:axId val="612691584"/>
+        <c:axId val="1564682997"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1556014590"/>
+        <c:axId val="612691584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4336,10 +4336,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="787541410"/>
+        <c:crossAx val="1564682997"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="787541410"/>
+        <c:axId val="1564682997"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4414,7 +4414,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1556014590"/>
+        <c:crossAx val="612691584"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4506,11 +4506,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1042258091"/>
-        <c:axId val="760973779"/>
+        <c:axId val="55021387"/>
+        <c:axId val="69238661"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1042258091"/>
+        <c:axId val="55021387"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4562,10 +4562,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="760973779"/>
+        <c:crossAx val="69238661"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="760973779"/>
+        <c:axId val="69238661"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4640,7 +4640,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1042258091"/>
+        <c:crossAx val="55021387"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4732,11 +4732,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="360531558"/>
-        <c:axId val="2079196675"/>
+        <c:axId val="989583131"/>
+        <c:axId val="961898556"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="360531558"/>
+        <c:axId val="989583131"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4788,10 +4788,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2079196675"/>
+        <c:crossAx val="961898556"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079196675"/>
+        <c:axId val="961898556"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4866,7 +4866,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360531558"/>
+        <c:crossAx val="989583131"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4958,11 +4958,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1535037134"/>
-        <c:axId val="1818354050"/>
+        <c:axId val="1418253012"/>
+        <c:axId val="395107719"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1535037134"/>
+        <c:axId val="1418253012"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5014,10 +5014,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1818354050"/>
+        <c:crossAx val="395107719"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1818354050"/>
+        <c:axId val="395107719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5092,7 +5092,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1535037134"/>
+        <c:crossAx val="1418253012"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5184,11 +5184,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1089878732"/>
-        <c:axId val="2049649593"/>
+        <c:axId val="1246746820"/>
+        <c:axId val="971110641"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1089878732"/>
+        <c:axId val="1246746820"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5240,10 +5240,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2049649593"/>
+        <c:crossAx val="971110641"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2049649593"/>
+        <c:axId val="971110641"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5318,7 +5318,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1089878732"/>
+        <c:crossAx val="1246746820"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5410,11 +5410,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1000119838"/>
-        <c:axId val="107282452"/>
+        <c:axId val="1134282364"/>
+        <c:axId val="1346074522"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1000119838"/>
+        <c:axId val="1134282364"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5466,10 +5466,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107282452"/>
+        <c:crossAx val="1346074522"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107282452"/>
+        <c:axId val="1346074522"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5544,7 +5544,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1000119838"/>
+        <c:crossAx val="1134282364"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>